<commit_message>
[utilities - schedule script] Changed color of one worker for readability, added additional student worker
</commit_message>
<xml_diff>
--- a/schedule-script/2023_Spring_Semester_Schedule1.xlsx
+++ b/schedule-script/2023_Spring_Semester_Schedule1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jophals/Dropbox (ASU)/Mac/Desktop/Py_root/utilities/schedule-script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6FDDCD87-D411-FF4E-9234-7E27AEBD65C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{55024B8B-B0A6-A84F-88F0-0D2A149E3ADD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="51200" yWindow="1580" windowWidth="51200" windowHeight="28800" xr2:uid="{C0155330-2702-4B7E-8643-5439E9035E99}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
   <si>
     <t>name</t>
   </si>
@@ -135,6 +135,9 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Ajay</t>
   </si>
 </sst>
 </file>
@@ -515,8 +518,8 @@
   <dimension ref="A1:V17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K5" sqref="K5"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1021,24 +1024,46 @@
       <c r="T12" s="1"/>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
+      <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13">
+        <v>15</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0.375</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0.5</v>
+      </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
+      <c r="K13" s="1">
+        <v>0.375</v>
+      </c>
+      <c r="L13" s="1">
+        <v>0.5</v>
+      </c>
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
-      <c r="P13" s="3"/>
+      <c r="O13" s="1">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="P13" s="3">
+        <v>0.47916666666666669</v>
+      </c>
       <c r="Q13" s="3"/>
       <c r="R13" s="3"/>
-      <c r="S13" s="3"/>
-      <c r="T13" s="3"/>
+      <c r="S13" s="1">
+        <v>0.375</v>
+      </c>
+      <c r="T13" s="3">
+        <v>0.64583333333333337</v>
+      </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="C14" s="1"/>

</xml_diff>